<commit_message>
Chg home image etc.
</commit_message>
<xml_diff>
--- a/doc/業務用アプリの例.xlsx
+++ b/doc/業務用アプリの例.xlsx
@@ -15,7 +15,8 @@
     <sheet name="営業支援" sheetId="1" r:id="rId1"/>
     <sheet name="施工支援（工務店）" sheetId="3" r:id="rId2"/>
     <sheet name="施工支援（）" sheetId="2" r:id="rId3"/>
-    <sheet name="画面構成" sheetId="4" r:id="rId4"/>
+    <sheet name="UX（小売）" sheetId="5" r:id="rId4"/>
+    <sheet name="画面構成" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>2015.7.14　吉田</t>
     <rPh sb="10" eb="12">
@@ -62,6 +63,47 @@
     <t>標準UX Flow</t>
     <rPh sb="0" eb="2">
       <t>ヒョウジュン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.1　店舗購入</t>
+    <rPh sb="4" eb="6">
+      <t>テンポ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>コウニュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>顧客</t>
+    <rPh sb="0" eb="2">
+      <t>コキャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>売り子</t>
+    <rPh sb="0" eb="1">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>システム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１．販売に関するUX</t>
+    <rPh sb="2" eb="4">
+      <t>ハンバイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>カン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -104,12 +146,129 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -118,11 +277,38 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -24344,6 +24530,2556 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="角丸四角形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="1190625"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>品物を持ってレジに行き、販売員に渡す</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="角丸四角形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2152650" y="1200150"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>金額を</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>POS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>（レジ）に入力する</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="角丸四角形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2114550" y="3462336"/>
+          <a:ext cx="1476375" cy="523876"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>入力完了キーを押す</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>108346</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>54761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1584721</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>64287</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="角丸四角形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2132409" y="4888699"/>
+          <a:ext cx="1476375" cy="527447"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>顧客に金額を伝える</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>103583</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>92862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1579958</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>102388</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="角丸四角形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2122883" y="5579262"/>
+          <a:ext cx="1476375" cy="523876"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>品物を包装する</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>165496</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>169062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1641871</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>7137</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="角丸四角形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="460771" y="5484012"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>支払いの準備をする</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="角丸四角形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3867150" y="1800225"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>販売トランザクションを開始する</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="角丸四角形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="2524125"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>入力された商品と金額を記録する</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>92866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>102391</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="角丸四角形 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3912394" y="4063600"/>
+          <a:ext cx="1476375" cy="527447"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>消費税を加えて合計金額を表示する</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="カギ線コネクタ 11"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="1452563"/>
+          <a:ext cx="285750" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>862013</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="カギ線コネクタ 13"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="8" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3629025" y="1462088"/>
+          <a:ext cx="976313" cy="338137"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>862013</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>871538</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="カギ線コネクタ 16"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="9" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4510088" y="2419349"/>
+          <a:ext cx="200025" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>833438</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>871538</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="カギ線コネクタ 19"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3526633" y="2374106"/>
+          <a:ext cx="414336" cy="1762125"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>900113</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>92866</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="カギ線コネクタ 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="10" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3590925" y="3724274"/>
+          <a:ext cx="1052513" cy="311942"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>846534</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>102392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>900113</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>54762</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="カギ線コネクタ 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3611764" y="3849881"/>
+          <a:ext cx="297652" cy="1779985"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>841772</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>64287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>846535</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>92862</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="カギ線コネクタ 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2763441" y="5476868"/>
+          <a:ext cx="200025" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>903685</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>145248</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>108347</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>169061</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="カギ線コネクタ 34"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="1"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1198960" y="5117298"/>
+          <a:ext cx="928687" cy="366713"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>113108</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>111912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1589483</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>121438</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="角丸四角形 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2132408" y="6455562"/>
+          <a:ext cx="1476375" cy="523876"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>品物を手渡す</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>165496</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>102387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1641871</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>111912</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="角丸四角形 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="460771" y="6960387"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>品物を受け取る</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>841770</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>102388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>851295</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>111912</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="カギ線コネクタ 39"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="38" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2689621" y="6274587"/>
+          <a:ext cx="352424" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>903685</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>30949</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>113109</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>102386</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="カギ線コネクタ 42"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="38" idx="1"/>
+          <a:endCxn id="39" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1198960" y="6717499"/>
+          <a:ext cx="933449" cy="242887"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>175021</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>7137</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1651396</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>16662</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="角丸四角形 45"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="470296" y="7722387"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>代金を支払う</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>903684</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>111911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>913209</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>7136</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="カギ線コネクタ 46"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="39" idx="2"/>
+          <a:endCxn id="46" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1084659" y="7598561"/>
+          <a:ext cx="238125" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>141683</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>83337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1618058</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>92863</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="角丸四角形 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2160983" y="8141487"/>
+          <a:ext cx="1476375" cy="523876"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>受取り金額を確認する</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1651396</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>97625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>879871</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>83337</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="カギ線コネクタ 50"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="3"/>
+          <a:endCxn id="50" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1946671" y="7984325"/>
+          <a:ext cx="952500" cy="157162"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>151208</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>111912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1627583</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>121438</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="角丸四角形 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2170508" y="8855862"/>
+          <a:ext cx="1476375" cy="523876"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>受取り金額を入力する</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>879871</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>92862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>889396</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>111911</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="カギ線コネクタ 54"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="2"/>
+          <a:endCxn id="54" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2808684" y="8755849"/>
+          <a:ext cx="190499" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>92866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>102391</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="角丸四角形 57"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3857625" y="9351166"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>おつりを計算する</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1627583</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>30950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>852488</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>92866</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="カギ線コネクタ 58"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="54" idx="3"/>
+          <a:endCxn id="58" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3646883" y="9117800"/>
+          <a:ext cx="948930" cy="233366"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>140491</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>150016</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="角丸四角形 62"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3857625" y="10084591"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>レシートを印刷する</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>846138</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>108741</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>858838</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>146841</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="カギ線コネクタ 63"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="58" idx="2"/>
+          <a:endCxn id="63" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4491038" y="9979816"/>
+          <a:ext cx="209550" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>141683</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>64287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1618058</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>73813</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="角丸四角形 66"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2160983" y="10522737"/>
+          <a:ext cx="1476375" cy="523876"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>入金しおつりとレシートを渡す</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>879871</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>59529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>64287</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="カギ線コネクタ 67"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="63" idx="1"/>
+          <a:endCxn id="67" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2899171" y="10346529"/>
+          <a:ext cx="958454" cy="176208"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>136921</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>26187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1613296</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>35712</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="角丸四角形 70"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="432196" y="10998987"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>おつりとレシートを受け取る</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>875110</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>154775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>141684</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>26187</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="カギ線コネクタ 71"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="67" idx="1"/>
+          <a:endCxn id="71" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1170385" y="10784675"/>
+          <a:ext cx="990599" cy="214312"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>54766</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>64291</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="角丸四角形 74"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3857625" y="11046616"/>
+          <a:ext cx="1476375" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>販売トランザクションを終了する</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>846138</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>156366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>858838</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>61116</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="カギ線コネクタ 75"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="63" idx="2"/>
+          <a:endCxn id="75" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4386263" y="10837066"/>
+          <a:ext cx="419100" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="円柱 78"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6067425" y="10820400"/>
+          <a:ext cx="1638300" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>販売ＤＢ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>145254</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="カギ線コネクタ 80"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="75" idx="3"/>
+          <a:endCxn id="79" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5334000" y="11306175"/>
+          <a:ext cx="733425" cy="2379"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="円柱 83"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8315325" y="9439275"/>
+          <a:ext cx="1638300" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>仕訳ＤＢ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>145254</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="カギ線コネクタ 84"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="75" idx="3"/>
+          <a:endCxn id="84" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5334000" y="9925050"/>
+          <a:ext cx="2981325" cy="1383504"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 12301"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="円柱 87"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10639425" y="8620125"/>
+          <a:ext cx="1638300" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>総勘定元帳ＤＢ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="カギ線コネクタ 88"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="84" idx="4"/>
+          <a:endCxn id="88" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9953625" y="9105900"/>
+          <a:ext cx="685800" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="円柱 95"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="12011025"/>
+          <a:ext cx="1638300" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>在庫ＤＢ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>145254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="カギ線コネクタ 96"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="75" idx="3"/>
+          <a:endCxn id="96" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="11308554"/>
+          <a:ext cx="742950" cy="1188246"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="角丸四角形 100"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8048625" y="7400925"/>
+          <a:ext cx="5057775" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 5173"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>会計機能</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="角丸四角形 101"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5886451" y="10153650"/>
+          <a:ext cx="1981200" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 5173"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>販売管理機能</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -28327,10 +31063,370 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="1.875" customWidth="1"/>
+    <col min="3" max="6" width="22.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="2:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C23" s="3"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C25" s="3"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C27" s="3"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C28" s="3"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C29" s="3"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C30" s="3"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C31" s="3"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C33" s="3"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C34" s="3"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C35" s="3"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C37" s="3"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C38" s="3"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C39" s="3"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C40" s="3"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C41" s="3"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C42" s="3"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C43" s="3"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C44" s="3"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C45" s="3"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C46" s="3"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C47" s="3"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C49" s="3"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C50" s="3"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C51" s="3"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C52" s="3"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C53" s="3"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C54" s="3"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C55" s="3"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C56" s="3"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C57" s="3"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C58" s="3"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C59" s="3"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C60" s="3"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C61" s="3"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C62" s="3"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C63" s="3"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C64" s="3"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C65" s="3"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C66" s="3"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C67" s="3"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C68" s="3"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="5"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>